<commit_message>
Start work on alt
</commit_message>
<xml_diff>
--- a/CH-113 Manage Duplicate Values.xlsx
+++ b/CH-113 Manage Duplicate Values.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AA0F931-2D83-424B-8492-E2E8EC89FA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746D6063-5E08-4C96-9179-43B90AAA3874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="14100" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Question</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>108-2-1</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/feed/update/urn:li:activity:7240826648583962625/</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -622,7 +625,9 @@
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>

</xml_diff>

<commit_message>
Going through Alt1 as example
</commit_message>
<xml_diff>
--- a/CH-113 Manage Duplicate Values.xlsx
+++ b/CH-113 Manage Duplicate Values.xlsx
@@ -8,19 +8,55 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746D6063-5E08-4C96-9179-43B90AAA3874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719171D5-5F02-45C9-BC4D-A34365503326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Alt1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>Question</t>
   </si>
@@ -401,6 +437,166 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3809999" cy="3581398"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Shape 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F610520-37B9-4806-9F82-1AEC9C5C2C4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1474470" y="0"/>
+          <a:ext cx="3809999" cy="3581398"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 12134"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="1C3052"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+          <a:headEnd type="none" w="sm" len="sm"/>
+          <a:tailEnd type="none" w="sm" len="sm"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr spcFirstLastPara="1" wrap="square" lIns="91425" tIns="45700" rIns="91425" bIns="45700" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" rtl="0">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+              <a:ea typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+              <a:sym typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Challenge 113: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+              <a:ea typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+              <a:sym typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Duplicate Values</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+              <a:ea typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+              <a:sym typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" rtl="0">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:br>
+            <a:rPr lang="en-US" sz="1600" b="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+              <a:ea typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+              <a:sym typeface="Times New Roman"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1600" b="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+              <a:ea typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+              <a:sym typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Consider the IDs in the question table. For duplicate values, add two numbers separated by a hyphen. The first number indicates the repetition set, and the second number indicates the occurrence of that ID within that set.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" rtl="0">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1600" b="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+              <a:ea typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+              <a:sym typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>For example, if ID 100 appears in row 14 as part of the third set of occurrences ID 100 and is the only occurrence in that set, it would be changed to 100-3-1.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -597,13 +793,40 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{08D9F231-B6EF-42E8-9026-6F55EEAC23A1}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1831,4 +2054,1321 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99FAF68-9427-422D-903A-87720E4DCFAE}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:L1000"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="8.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="9">
+        <v>100</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="9">
+        <v>100</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="7">
+        <v>102</v>
+      </c>
+      <c r="D5" s="7">
+        <v>102</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="B6" s="7">
+        <v>103</v>
+      </c>
+      <c r="D6" s="7">
+        <v>103</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="9">
+        <v>100</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="9">
+        <v>100</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="7">
+        <v>107</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="7">
+        <v>107</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="7">
+        <v>108</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="7">
+        <v>108</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="7">
+        <v>108</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="B14" s="9">
+        <v>100</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="8">
+        <v>108</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" t="str" cm="1">
+        <f t="array" ref="B21:B34">_xlfn.LET(
+    _xlpm.p, B3:B15,
+    _xlpm.u, _xlfn.UNIQUE(_xlpm.p),
+    _xlpm.r, ROW(_xlpm.p),
+    _xlpm.b, _xlfn.REDUCE(
+        0,
+        _xlpm.u,
+        _xlfn.LAMBDA(_xlpm.i,_xlpm.x,
+            _xlpm.i + _xlfn.SCAN(, N(_xlpm.p = _xlpm.x), _xlfn.LAMBDA(_xlpm.j,_xlpm.y, _xlpm.y * (_xlpm.j + _xlpm.y)))
+        )
+    ),
+    _xlpm.z, _xlpm.p &amp; -_xlpm.b,
+    _xlfn.VSTACK(
+        B2,
+        IF(
+            COUNTIF(_xlpm.p, _xlpm.p) - 1,
+            _xlpm.p &amp;
+                -MMULT(
+                    (_xlpm.z = _xlfn.TOROW(_xlpm.z)) * (_xlpm.r &gt;= _xlfn.TOROW(_xlpm.r)),
+                    _xlpm.r ^ 0
+                ) &amp; -_xlpm.b,
+            _xlpm.p
+        )
+    )
+)</f>
+        <v>Product ID</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" t="str">
+        <v>100-1-1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" t="str">
+        <v>100-1-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" t="str">
+        <v>100-2-1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" t="str">
+        <v>100-2-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" t="str">
+        <v>107-1-1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" t="str">
+        <v>107-1-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" t="str">
+        <v>108-1-1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" t="str">
+        <v>108-1-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" t="str">
+        <v>108-1-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" t="str">
+        <v>100-3-1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" t="str">
+        <v>108-2-1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Okay, I understand the alt.
</commit_message>
<xml_diff>
--- a/CH-113 Manage Duplicate Values.xlsx
+++ b/CH-113 Manage Duplicate Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719171D5-5F02-45C9-BC4D-A34365503326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA1E2AF-41FE-40B7-9C41-5092469A2969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +142,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -243,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -260,6 +267,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,7 +803,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="267" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -807,7 +815,9 @@
   <we:alternateReferences>
     <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
   </we:alternateReferences>
-  <we:properties/>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{5EE0D513-A610-4BC4-85E3-3A5F102D64ED}&quot;}"/>
+  </we:properties>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
@@ -2061,8 +2071,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2304,8 +2314,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F16" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(G21)</f>
+        <v>=REDUCE(0, E21#, LAMBDA(i,x, i + SCAN(, N(B3:B15 = x), LAMBDA(j,y, y * (j + y)))))</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" t="str" cm="1">
         <f t="array" ref="B21:B34">_xlfn.LET(
     _xlpm.p, B3:B15,
@@ -2334,86 +2350,222 @@
 )</f>
         <v>Product ID</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" cm="1">
+        <f t="array" ref="C21:C33">_xlfn.LET(_xlpm.p, B3:B15, _xlpm.u, _xlfn.UNIQUE(_xlpm.p), _xlpm.r, ROW(_xlpm.p), _xlpm.b, _xlfn.REDUCE(0, _xlpm.u, _xlfn.LAMBDA(_xlpm.i,_xlpm.x, _xlpm.i + _xlfn.SCAN(, N(_xlpm.p = _xlpm.x), _xlfn.LAMBDA(_xlpm.j,_xlpm.y, _xlpm.y * (_xlpm.j + _xlpm.y))))), _xlpm.z, _xlpm.p &amp; -_xlpm.b, _xlpm.b)</f>
+        <v>1</v>
+      </c>
+      <c r="E21" cm="1">
+        <f t="array" ref="E21:E25">_xlfn.UNIQUE(B3:B15)</f>
+        <v>100</v>
+      </c>
+      <c r="G21" s="10" cm="1">
+        <f t="array" ref="G21:G33">_xlfn.REDUCE(0,_xlfn.ANCHORARRAY( E21), _xlfn.LAMBDA(_xlpm.i,_xlpm.x, _xlpm.i + _xlfn.SCAN(, N(B3:B15 = _xlpm.x), _xlfn.LAMBDA(_xlpm.j,_xlpm.y, _xlpm.y * (_xlpm.j + _xlpm.y)))))</f>
+        <v>1</v>
+      </c>
+      <c r="I21" cm="1">
+        <f t="array" ref="I21:I33">_xlfn.SCAN(,N(B3:B15=100),_xlfn.LAMBDA(_xlpm.j,_xlpm.y,_xlpm.y*(_xlpm.j+_xlpm.y)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <v>100-1-1</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>102</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <v>100-1-2</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>103</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>102</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>107</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>103</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>108</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <v>100-2-1</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <v>100-2-2</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <v>107-1-1</v>
       </c>
-    </row>
-    <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" t="str">
         <v>107-1-2</v>
       </c>
-    </row>
-    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" t="str">
         <v>108-1-1</v>
       </c>
-    </row>
-    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <v>108-1-2</v>
       </c>
-    </row>
-    <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <v>108-1-3</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <v>100-3-1</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <v>108-2-1</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3371,4 +3523,16 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EE0D513-A610-4BC4-85E3-3A5F102D64ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>